<commit_message>
width of columns updated to 16
</commit_message>
<xml_diff>
--- a/section2/ExcelHomework.xlsx
+++ b/section2/ExcelHomework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsong\Code\SavvyCoders\Homework\section2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCBEB47-FD86-4D89-9BFA-AF976088BD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D40B368-0809-40AA-AA4B-C33D2F2770A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="16" r:id="rId5"/>
+    <pivotCache cacheId="17" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -567,7 +567,7 @@
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -702,7 +702,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -711,238 +711,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="72">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <b val="0"/>
@@ -1120,17 +889,80 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color indexed="64"/>
-        </top>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -6771,7 +6603,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{689130F7-F52D-4A47-BD5F-BAB04971381C}" name="PivotTable7" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{689130F7-F52D-4A47-BD5F-BAB04971381C}" name="PivotTable7" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:E7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField numFmtId="14" showAll="0"/>
@@ -6934,16 +6766,16 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of Tax Inclusive Amount" fld="4" baseField="0" baseItem="0" numFmtId="168"/>
+    <dataField name="Sum of Tax Inclusive Amount" fld="4" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="58">
+    <format dxfId="15">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="57">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="55">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -7009,18 +6841,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{77EEBAA1-C28C-442D-AB35-2F8E43797D12}" name="Table2" displayName="Table2" ref="A2:I210" totalsRowShown="0" headerRowDxfId="59" dataDxfId="60" headerRowBorderDxfId="70" tableBorderDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{77EEBAA1-C28C-442D-AB35-2F8E43797D12}" name="Table2" displayName="Table2" ref="A2:I210" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
   <autoFilter ref="A2:I210" xr:uid="{77EEBAA1-C28C-442D-AB35-2F8E43797D12}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{3B6080E7-7D06-436E-8572-92B71DEA28E1}" name="Document Date" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{C68F8EEB-7452-4924-BAE2-BD5C94721B13}" name="Supplier" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{A1FF7F87-625B-40B0-9B64-9DBDBCEC589D}" name="Reference" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{8CB55289-C261-483D-B192-8143D4E5A23B}" name="Description" dataDxfId="66"/>
-    <tableColumn id="5" xr3:uid="{AB9F19A8-435A-49DE-B449-C986C1C14C0A}" name="Tax Inclusive Amount" dataDxfId="65" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{44D31B54-0986-413C-8A7D-6D874E5360DA}" name="Column1" dataDxfId="64"/>
-    <tableColumn id="7" xr3:uid="{B5C6D540-AF15-4C53-AF20-09F3E7DB0FF4}" name="Bank Code" dataDxfId="63"/>
-    <tableColumn id="8" xr3:uid="{A7FA3217-C633-447D-B8E8-37DAECABF89D}" name="Account Code" dataDxfId="62"/>
-    <tableColumn id="9" xr3:uid="{618F1AF5-7693-4BFD-9E3F-641CAD72F47E}" name="Payment Date" dataDxfId="61"/>
+    <tableColumn id="1" xr3:uid="{3B6080E7-7D06-436E-8572-92B71DEA28E1}" name="Document Date" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{C68F8EEB-7452-4924-BAE2-BD5C94721B13}" name="Supplier" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{A1FF7F87-625B-40B0-9B64-9DBDBCEC589D}" name="Reference" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{8CB55289-C261-483D-B192-8143D4E5A23B}" name="Description" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{AB9F19A8-435A-49DE-B449-C986C1C14C0A}" name="Tax Inclusive Amount" dataDxfId="4" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{44D31B54-0986-413C-8A7D-6D874E5360DA}" name="Column1" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{B5C6D540-AF15-4C53-AF20-09F3E7DB0FF4}" name="Bank Code" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{A7FA3217-C633-447D-B8E8-37DAECABF89D}" name="Account Code" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{618F1AF5-7693-4BFD-9E3F-641CAD72F47E}" name="Payment Date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7339,16 +7171,14 @@
   <dimension ref="A3:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" style="22" customWidth="1"/>
+    <col min="3" max="5" width="16.6328125" customWidth="1"/>
     <col min="6" max="6" width="3.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.6328125" bestFit="1" customWidth="1"/>

</xml_diff>